<commit_message>
Edit DataClassification in spreadsheet
</commit_message>
<xml_diff>
--- a/resources/Order Events.xlsx
+++ b/resources/Order Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcollingwood/Projects/datacontract_models/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B1D7FE-5198-CF4A-9800-076E0811F3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D327AAC-DBE2-3B45-971B-962A88592637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$26</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="87">
   <si>
     <t>Event</t>
   </si>
@@ -275,6 +275,15 @@
   </si>
   <si>
     <t>Globally Unique</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Private</t>
   </si>
 </sst>
 </file>
@@ -554,11 +563,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AJ26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -567,16 +576,16 @@
     <col min="3" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="8" width="14" customWidth="1"/>
-    <col min="9" max="11" width="22.5" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
-    <col min="15" max="17" width="14.83203125" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="22.5" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="16" max="18" width="14.83203125" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" customWidth="1"/>
+    <col min="21" max="21" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,33 +620,35 @@
         <v>82</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
@@ -652,8 +663,9 @@
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
-    </row>
-    <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AJ1" s="2"/>
+    </row>
+    <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -686,34 +698,37 @@
         <v>83</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="b">
-        <v>1</v>
+      <c r="P2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
@@ -730,34 +745,37 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="3" t="b">
-        <v>1</v>
+      <c r="P3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
@@ -776,34 +794,37 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="3" t="b">
-        <v>1</v>
+      <c r="P4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
@@ -817,24 +838,25 @@
         <v>38</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="O5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="3"/>
+      <c r="S5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E6" s="3" t="s">
         <v>40</v>
       </c>
@@ -853,34 +875,37 @@
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="3" t="b">
-        <v>1</v>
+      <c r="P6" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
         <v>44</v>
@@ -893,23 +918,24 @@
         <v>45</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="N7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="3" t="s">
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -929,26 +955,27 @@
         <v>49</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="3"/>
+      <c r="M8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="3" t="b">
-        <v>0</v>
+      <c r="P8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q8" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
         <v>51</v>
@@ -961,26 +988,27 @@
         <v>52</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="3" t="b">
-        <v>1</v>
+      <c r="P9" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q9" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -1011,25 +1039,28 @@
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="3" t="b">
-        <v>1</v>
+      <c r="P10" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q10" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R10" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>58</v>
@@ -1042,26 +1073,27 @@
         <v>59</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="3" t="b">
-        <v>1</v>
+      <c r="P11" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q11" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
         <v>62</v>
@@ -1074,26 +1106,27 @@
         <v>63</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="3" t="b">
-        <v>1</v>
+      <c r="P12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q12" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1112,34 +1145,37 @@
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="3" t="b">
-        <v>1</v>
+      <c r="P13" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R13" s="3" t="s">
+      <c r="R13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1162,34 +1198,37 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="O14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="3" t="b">
-        <v>1</v>
+      <c r="P14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="T14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1208,34 +1247,37 @@
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="O15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="3" t="b">
-        <v>1</v>
+      <c r="P15" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="3" t="s">
+      <c r="T15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T15" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>44</v>
@@ -1248,23 +1290,24 @@
         <v>45</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="N16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="3" t="s">
+      <c r="R16" s="3"/>
+      <c r="S16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S16" s="3" t="s">
+      <c r="T16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T16" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
         <v>47</v>
@@ -1279,26 +1322,27 @@
         <v>49</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="O17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P17" s="3" t="b">
-        <v>0</v>
+      <c r="P17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q17" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R17" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
         <v>51</v>
@@ -1311,26 +1355,27 @@
         <v>52</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="3"/>
+      <c r="M18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P18" s="3" t="b">
-        <v>1</v>
+      <c r="P18" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q18" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
         <v>66</v>
@@ -1343,26 +1388,27 @@
         <v>59</v>
       </c>
       <c r="K19" s="3"/>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="3"/>
+      <c r="M19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="O19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="3" t="b">
-        <v>1</v>
+      <c r="P19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q19" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R19" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
         <v>68</v>
@@ -1375,26 +1421,27 @@
         <v>59</v>
       </c>
       <c r="K20" s="3"/>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="O20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P20" s="3" t="b">
-        <v>1</v>
+      <c r="P20" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q20" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -1425,34 +1472,37 @@
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="N21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="O21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21" s="3" t="b">
-        <v>1</v>
+      <c r="P21" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R21" s="3" t="s">
+      <c r="R21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="T21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
@@ -1467,34 +1517,37 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="O22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P22" s="3" t="b">
-        <v>1</v>
+      <c r="P22" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="S22" s="3" t="s">
+      <c r="T22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E23" s="3" t="s">
         <v>71</v>
       </c>
@@ -1513,34 +1566,37 @@
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="O23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P23" s="3" t="b">
-        <v>1</v>
+      <c r="P23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q23" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R23" s="3" t="s">
+      <c r="R23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S23" s="3" t="s">
+      <c r="T23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T23" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
@@ -1554,26 +1610,27 @@
         <v>38</v>
       </c>
       <c r="K24" s="3"/>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="3"/>
+      <c r="M24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="O24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P24" s="3" t="b">
-        <v>1</v>
+      <c r="P24" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q24" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E25" s="3" t="s">
         <v>72</v>
       </c>
@@ -1592,34 +1649,37 @@
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="N25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="O25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P25" s="3" t="b">
-        <v>1</v>
+      <c r="P25" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R25" s="3" t="s">
+      <c r="R25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S25" s="3" t="s">
+      <c r="T25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T25" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1631,27 +1691,28 @@
         <v>38</v>
       </c>
       <c r="K26" s="3"/>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="3"/>
+      <c r="M26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="O26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P26" s="3" t="b">
-        <v>1</v>
+      <c r="P26" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="Q26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R26" s="3" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
additional numeric and temporal schema types
</commit_message>
<xml_diff>
--- a/resources/Order Events.xlsx
+++ b/resources/Order Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcollingwood/Projects/datacontract_models/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D327AAC-DBE2-3B45-971B-962A88592637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE18C08-073F-294A-9F74-28DEC9829BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="86">
   <si>
     <t>Event</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>Attribute Cardinality</t>
-  </si>
-  <si>
     <t>Semantic Type</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Variation</t>
   </si>
   <si>
-    <t>Zero or Many</t>
-  </si>
-  <si>
     <t>Product Variation</t>
   </si>
   <si>
@@ -284,6 +278,9 @@
   </si>
   <si>
     <t>Private</t>
+  </si>
+  <si>
+    <t>Attribute Timing</t>
   </si>
 </sst>
 </file>
@@ -567,7 +564,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -590,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -608,46 +605,46 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
@@ -667,272 +664,260 @@
     </row>
     <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="U2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="T3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="U4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="U6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -943,30 +928,28 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="3" t="b">
         <v>0</v>
@@ -978,28 +961,26 @@
     <row r="9" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="3" t="b">
         <v>1</v>
@@ -1010,48 +991,46 @@
     </row>
     <row r="10" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="3" t="b">
         <v>1</v>
@@ -1063,28 +1042,26 @@
     <row r="11" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="3" t="b">
         <v>1</v>
@@ -1096,28 +1073,26 @@
     <row r="12" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q12" s="3" t="b">
         <v>1</v>
@@ -1128,51 +1103,49 @@
     </row>
     <row r="13" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="O13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S13" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="U13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1181,159 +1154,151 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="U14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="U15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q17" s="3" t="b">
         <v>0</v>
@@ -1345,28 +1310,26 @@
     <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q18" s="3" t="b">
         <v>1</v>
@@ -1378,28 +1341,26 @@
     <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q19" s="3" t="b">
         <v>1</v>
@@ -1411,28 +1372,26 @@
     <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q20" s="3" t="b">
         <v>1</v>
@@ -1443,185 +1402,177 @@
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="O21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S21" s="3" t="s">
+      <c r="T21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T21" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="U21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="O22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="T22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E23" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="T23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q24" s="3" t="b">
         <v>1</v>
@@ -1632,77 +1583,73 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E25" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="T25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G26" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q26" s="3" t="b">
         <v>1</v>

</xml_diff>